<commit_message>
Updated to better use the 1819 datalocks, and to use the V1 commitments Also writing more output
</commit_message>
<xml_diff>
--- a/src/SFA.DAS.Payments.Contingency/Template/Contingency.xlsx
+++ b/src/SFA.DAS.Payments.Contingency/Template/Contingency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\das-payments-v2-verification\src\SFA.DAS.Payments.Contingency\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB959117-4E44-47F9-A79A-7ADCB25D0E5B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15317782-E012-4B3A-81F2-0D9BBB0E2AC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{A67A014B-8CE1-4811-965E-6D546D03FD24}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="6" xr2:uid="{A67A014B-8CE1-4811-965E-6D546D03FD24}"/>
   </bookViews>
   <sheets>
     <sheet name="Earnings" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="1920 Datalocks" sheetId="3" r:id="rId3"/>
     <sheet name="Final Amounts" sheetId="5" r:id="rId4"/>
     <sheet name="Summary" sheetId="6" r:id="rId5"/>
+    <sheet name="Raw Earnings" sheetId="7" r:id="rId6"/>
+    <sheet name="Raw 1819 Datalocks" sheetId="9" r:id="rId7"/>
+    <sheet name="Raw 1920 Datalocks" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
   <si>
     <t>Ukprn</t>
   </si>
@@ -58,6 +61,57 @@
   </si>
   <si>
     <t>Number of Paid learners</t>
+  </si>
+  <si>
+    <t>Transaction Type 1</t>
+  </si>
+  <si>
+    <t>TT 2</t>
+  </si>
+  <si>
+    <t>TT 3</t>
+  </si>
+  <si>
+    <t>TT 4</t>
+  </si>
+  <si>
+    <t>TT 5</t>
+  </si>
+  <si>
+    <t>TT 6</t>
+  </si>
+  <si>
+    <t>TT 7</t>
+  </si>
+  <si>
+    <t>TT 8</t>
+  </si>
+  <si>
+    <t>TT 9</t>
+  </si>
+  <si>
+    <t>TT 10</t>
+  </si>
+  <si>
+    <t>TT 11</t>
+  </si>
+  <si>
+    <t>TT 12</t>
+  </si>
+  <si>
+    <t>TT 13</t>
+  </si>
+  <si>
+    <t>TT 14</t>
+  </si>
+  <si>
+    <t>TT 15</t>
+  </si>
+  <si>
+    <t>TT 16</t>
+  </si>
+  <si>
+    <t>Uln</t>
   </si>
 </sst>
 </file>
@@ -440,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4CF6A8-09F9-4305-A8ED-1292A97BDDBD}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -539,7 +593,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -603,4 +657,244 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD908C42-CA2A-4FC6-BFE1-B1D47A280042}">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="18.61328125" customWidth="1"/>
+    <col min="4" max="4" width="18.07421875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABB18A6-2728-408F-B39B-1D637B37ED2C}">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="18.61328125" customWidth="1"/>
+    <col min="4" max="4" width="18.07421875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFB9ED9-8B05-4835-8E4E-D902C20B8878}">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="18.61328125" customWidth="1"/>
+    <col min="4" max="4" width="18.07421875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed act1 co-investment multiplier Added output for tt 1-3 and 4-16 Does data match for 1920 on both the 'full' commitment as well as Ukpnr/Uln only
</commit_message>
<xml_diff>
--- a/src/SFA.DAS.Payments.Contingency/Template/Contingency.xlsx
+++ b/src/SFA.DAS.Payments.Contingency/Template/Contingency.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\das-payments-v2-verification\src\SFA.DAS.Payments.Contingency\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15317782-E012-4B3A-81F2-0D9BBB0E2AC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3B56BE-FD8C-40C6-9466-8C0A47C17CA9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="6" xr2:uid="{A67A014B-8CE1-4811-965E-6D546D03FD24}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" firstSheet="3" activeTab="6" xr2:uid="{A67A014B-8CE1-4811-965E-6D546D03FD24}"/>
   </bookViews>
   <sheets>
     <sheet name="Earnings" sheetId="1" r:id="rId1"/>
     <sheet name="1819 Datalocks" sheetId="2" r:id="rId2"/>
-    <sheet name="1920 Datalocks" sheetId="3" r:id="rId3"/>
-    <sheet name="Final Amounts" sheetId="5" r:id="rId4"/>
-    <sheet name="Summary" sheetId="6" r:id="rId5"/>
-    <sheet name="Raw Earnings" sheetId="7" r:id="rId6"/>
-    <sheet name="Raw 1819 Datalocks" sheetId="9" r:id="rId7"/>
-    <sheet name="Raw 1920 Datalocks" sheetId="10" r:id="rId8"/>
+    <sheet name="1920 Datalocks (Full)" sheetId="12" r:id="rId3"/>
+    <sheet name="1920 Datalocks (Partial)" sheetId="3" r:id="rId4"/>
+    <sheet name="Final Amounts (Full)" sheetId="11" r:id="rId5"/>
+    <sheet name="Final Amounts (Partial)" sheetId="5" r:id="rId6"/>
+    <sheet name="Summary" sheetId="6" r:id="rId7"/>
+    <sheet name="Raw Earnings" sheetId="7" r:id="rId8"/>
+    <sheet name="Raw 1819 Datalocks" sheetId="9" r:id="rId9"/>
+    <sheet name="Raw 1920 Datalocks (Full)" sheetId="10" r:id="rId10"/>
+    <sheet name="Raw 1920 Datalocks (Partial)" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="16">
   <si>
     <t>Ukprn</t>
   </si>
@@ -63,63 +66,41 @@
     <t>Number of Paid learners</t>
   </si>
   <si>
-    <t>Transaction Type 1</t>
-  </si>
-  <si>
-    <t>TT 2</t>
-  </si>
-  <si>
-    <t>TT 3</t>
-  </si>
-  <si>
-    <t>TT 4</t>
-  </si>
-  <si>
-    <t>TT 5</t>
-  </si>
-  <si>
-    <t>TT 6</t>
-  </si>
-  <si>
-    <t>TT 7</t>
-  </si>
-  <si>
-    <t>TT 8</t>
-  </si>
-  <si>
-    <t>TT 9</t>
-  </si>
-  <si>
-    <t>TT 10</t>
-  </si>
-  <si>
-    <t>TT 11</t>
-  </si>
-  <si>
-    <t>TT 12</t>
-  </si>
-  <si>
-    <t>TT 13</t>
-  </si>
-  <si>
-    <t>TT 14</t>
-  </si>
-  <si>
-    <t>TT 15</t>
-  </si>
-  <si>
-    <t>TT 16</t>
-  </si>
-  <si>
     <t>Uln</t>
+  </si>
+  <si>
+    <t>TT 1-3</t>
+  </si>
+  <si>
+    <t>TT 4-16</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>Number of Learners Removed
+1920 by matching everything</t>
+  </si>
+  <si>
+    <t>Number of learners removed
+1920 matching Ukprn and Uln only</t>
+  </si>
+  <si>
+    <t>Amount removed
+in 1920 (Full)</t>
+  </si>
+  <si>
+    <t>Amount removed
+in 1920 (Ukprn &amp; Uln)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -162,11 +143,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -177,8 +159,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -492,11 +484,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4CF6A8-09F9-4305-A8ED-1292A97BDDBD}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -506,7 +498,7 @@
     <col min="3" max="3" width="9.23046875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -516,6 +508,96 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFB9ED9-8B05-4835-8E4E-D902C20B8878}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="9.23046875" style="9"/>
+    <col min="3" max="3" width="18.61328125" customWidth="1"/>
+    <col min="4" max="4" width="18.07421875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6456F657-1B06-4386-877A-F9FAD0C966CB}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="9.23046875" style="9"/>
+    <col min="3" max="3" width="18.61328125" customWidth="1"/>
+    <col min="4" max="4" width="18.07421875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -525,11 +607,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A3EBC3-4635-4620-8B42-512DE1B13D73}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -539,7 +621,7 @@
     <col min="3" max="3" width="9.23046875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -549,6 +631,12 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -556,12 +644,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22971F7-7B96-42A6-A567-4A5D9F50D192}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3169127F-61B3-438A-9700-706EA62A7CD5}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -571,7 +659,7 @@
     <col min="3" max="3" width="9.23046875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -581,6 +669,12 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -588,12 +682,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A7ACBC-E4E5-44C2-B2F0-2E6552747512}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22971F7-7B96-42A6-A567-4A5D9F50D192}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -603,7 +697,7 @@
     <col min="3" max="3" width="9.23046875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -613,6 +707,12 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -620,72 +720,175 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB9BF56-870E-490B-A553-9EECD48D815F}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B695CA90-1D76-4287-BF29-727446556F12}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="15.53515625" customWidth="1"/>
-    <col min="2" max="2" width="19.15234375" customWidth="1"/>
-    <col min="3" max="3" width="20.53515625" customWidth="1"/>
-    <col min="4" max="4" width="30.3828125" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD908C42-CA2A-4FC6-BFE1-B1D47A280042}">
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="3" max="3" width="18.61328125" customWidth="1"/>
-    <col min="4" max="4" width="18.07421875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.15234375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="67.07421875" customWidth="1"/>
+    <col min="3" max="3" width="9.23046875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A7ACBC-E4E5-44C2-B2F0-2E6552747512}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.15234375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="67.07421875" customWidth="1"/>
+    <col min="3" max="3" width="9.23046875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB9BF56-870E-490B-A553-9EECD48D815F}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.53515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="19.15234375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.53515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.3828125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="24" style="7" customWidth="1"/>
+    <col min="6" max="6" width="26.84375" customWidth="1"/>
+    <col min="7" max="7" width="32.4609375" customWidth="1"/>
+    <col min="8" max="8" width="17.3828125" customWidth="1"/>
+    <col min="9" max="9" width="20.61328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="29.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD908C42-CA2A-4FC6-BFE1-B1D47A280042}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="9.23046875" style="9"/>
+    <col min="3" max="3" width="18.61328125" customWidth="1"/>
+    <col min="4" max="4" width="18.07421875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
@@ -693,45 +896,6 @@
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -739,33 +903,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABB18A6-2728-408F-B39B-1D637B37ED2C}">
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="9.23046875" style="9"/>
     <col min="3" max="3" width="18.61328125" customWidth="1"/>
-    <col min="4" max="4" width="18.07421875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <col min="4" max="4" width="18.07421875" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
@@ -773,128 +938,9 @@
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFB9ED9-8B05-4835-8E4E-D902C20B8878}">
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="3" max="3" width="18.61328125" customWidth="1"/>
-    <col min="4" max="4" width="18.07421875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>